<commit_message>
Test networkgraph Default Page
</commit_message>
<xml_diff>
--- a/Resource/โครงสร้างบริหารคุรุสภา.xlsx
+++ b/Resource/โครงสร้างบริหารคุรุสภา.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIT\KSP-BI\GIT\KSP-MIS\Resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\KSP-MIS\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC449337-816C-4BB6-BEEC-69E9E7F6AADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D419C61C-4442-466C-B175-416BAC3AA729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{E941F272-9114-47A2-B0CA-4CDD2C5755CF}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="40">
   <si>
     <t>กลุ่มพัฒนาระบบงาน</t>
   </si>
@@ -144,6 +142,15 @@
   </si>
   <si>
     <t>http://www.ksp.or.th/ksp2018/executives/</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>bbbbb</t>
+  </si>
+  <si>
+    <t>ccccc</t>
   </si>
 </sst>
 </file>
@@ -516,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EBF23D-BCCD-4E79-82A7-CA725B853A90}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G11" sqref="G11:K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -530,12 +537,12 @@
     <col min="4" max="4" width="31.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>32</v>
       </c>
@@ -543,7 +550,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
@@ -551,7 +558,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
@@ -559,178 +566,689 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C8" s="1"/>
       <c r="D8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C10" s="1"/>
       <c r="D10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" t="s">
+        <v>38</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C32" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C33" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="G34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.45">
       <c r="D35" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G37" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" t="s">
+        <v>38</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" t="s">
+        <v>38</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="G43" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>38</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>